<commit_message>
Chỉnh lại thông số wave 1-1
</commit_message>
<xml_diff>
--- a/Wave and Turn.xlsx
+++ b/Wave and Turn.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64C3877-01EE-4106-AF9E-12E41BA88B15}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60763A3-89E6-4DF2-8C19-36415FB29EA4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="19965" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8730" yWindow="3330" windowWidth="19965" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cặc" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>Wave</t>
   </si>
@@ -176,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -190,17 +190,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -208,7 +199,13 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -496,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E7:Q37"/>
+  <dimension ref="E7:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8:O32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +552,7 @@
       </c>
     </row>
     <row r="8" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="3">
@@ -580,15 +577,15 @@
         <v>0</v>
       </c>
       <c r="M8" s="3"/>
-      <c r="N8" s="5">
+      <c r="N8" s="8">
         <v>25</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="8">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E9" s="10"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="3">
         <v>2</v>
       </c>
@@ -611,14 +608,14 @@
         <v>0</v>
       </c>
       <c r="M9" s="3"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E10" s="10"/>
-      <c r="F10" s="5">
+      <c r="E10" s="7"/>
+      <c r="F10" s="8">
         <v>3</v>
       </c>
       <c r="G10" s="3">
@@ -639,13 +636,13 @@
       <c r="L10" s="3">
         <v>0</v>
       </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
     </row>
     <row r="11" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E11" s="10"/>
-      <c r="F11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="10"/>
       <c r="G11" s="3">
         <v>2</v>
       </c>
@@ -656,7 +653,7 @@
         <v>5</v>
       </c>
       <c r="J11" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K11" s="3">
         <v>0.5</v>
@@ -664,13 +661,13 @@
       <c r="L11" s="3">
         <v>0</v>
       </c>
-      <c r="M11" s="6"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
     </row>
     <row r="12" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E12" s="10"/>
-      <c r="F12" s="5">
+      <c r="E12" s="7"/>
+      <c r="F12" s="8">
         <v>4</v>
       </c>
       <c r="G12" s="3">
@@ -691,13 +688,13 @@
       <c r="L12" s="3">
         <v>0</v>
       </c>
-      <c r="M12" s="5"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
     </row>
     <row r="13" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E13" s="10"/>
-      <c r="F13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="10"/>
       <c r="G13" s="3">
         <v>2</v>
       </c>
@@ -708,7 +705,7 @@
         <v>3</v>
       </c>
       <c r="J13" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K13" s="3">
         <v>0.5</v>
@@ -716,17 +713,17 @@
       <c r="L13" s="3">
         <v>2</v>
       </c>
-      <c r="M13" s="6"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
     </row>
     <row r="14" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E14" s="10"/>
-      <c r="F14" s="5">
+      <c r="E14" s="7"/>
+      <c r="F14" s="9">
         <v>5</v>
       </c>
       <c r="G14" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>8</v>
@@ -735,163 +732,163 @@
         <v>25</v>
       </c>
       <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+    </row>
+    <row r="15" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E15" s="7"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="3">
         <v>3</v>
       </c>
-      <c r="K14" s="3">
-        <v>2</v>
-      </c>
-      <c r="L14" s="3">
-        <v>0</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-    </row>
-    <row r="15" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E15" s="10"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="3">
-        <v>2</v>
-      </c>
       <c r="H15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I15" s="3">
+        <v>20</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0</v>
+      </c>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+    </row>
+    <row r="16" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E16" s="7"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="3">
+        <v>4</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="3">
         <v>25</v>
       </c>
-      <c r="J15" s="3">
-        <v>0</v>
-      </c>
-      <c r="K15" s="3">
-        <v>1</v>
-      </c>
-      <c r="L15" s="3">
-        <v>0</v>
-      </c>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-    </row>
-    <row r="16" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E16" s="10"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="3">
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0</v>
+      </c>
+      <c r="M16" s="10"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+    </row>
+    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E17" s="7"/>
+      <c r="F17" s="8">
+        <v>6</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="3">
+        <v>10</v>
+      </c>
+      <c r="J17" s="3">
         <v>3</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I16" s="3">
-        <v>20</v>
-      </c>
-      <c r="J16" s="3">
-        <v>0</v>
-      </c>
-      <c r="K16" s="3">
-        <v>1</v>
-      </c>
-      <c r="L16" s="3">
-        <v>0</v>
-      </c>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-    </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E17" s="10"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="3">
-        <v>4</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" s="3">
-        <v>25</v>
-      </c>
-      <c r="J17" s="3">
-        <v>0</v>
-      </c>
       <c r="K17" s="3">
+        <v>1</v>
+      </c>
+      <c r="L17" s="3">
+        <v>0</v>
+      </c>
+      <c r="M17" s="8"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+    </row>
+    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E18" s="7"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="3">
+        <v>2</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="3">
+        <v>5</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3">
         <v>0.5</v>
       </c>
-      <c r="L17" s="3">
-        <v>0</v>
-      </c>
-      <c r="M17" s="6"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-    </row>
-    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E18" s="10"/>
-      <c r="F18" s="5">
-        <v>6</v>
-      </c>
-      <c r="G18" s="3">
-        <v>1</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18" s="3">
-        <v>10</v>
-      </c>
-      <c r="J18" s="3">
-        <v>2</v>
-      </c>
-      <c r="K18" s="3">
-        <v>1</v>
-      </c>
       <c r="L18" s="3">
         <v>0</v>
       </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
     </row>
     <row r="19" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E19" s="10"/>
-      <c r="F19" s="8"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="9">
+        <v>7</v>
+      </c>
       <c r="G19" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I19" s="3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J19" s="3">
         <v>2</v>
       </c>
       <c r="K19" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L19" s="3">
         <v>0</v>
       </c>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
     </row>
     <row r="20" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E20" s="10"/>
-      <c r="F20" s="8">
-        <v>7</v>
-      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="10"/>
       <c r="G20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I20" s="3">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="J20" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K20" s="3">
         <v>0.5</v>
@@ -899,21 +896,23 @@
       <c r="L20" s="3">
         <v>0</v>
       </c>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
     </row>
     <row r="21" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E21" s="10"/>
-      <c r="F21" s="6"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8">
+        <v>8</v>
+      </c>
       <c r="G21" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I21" s="3">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="J21" s="3">
         <v>2</v>
@@ -924,17 +923,15 @@
       <c r="L21" s="3">
         <v>0</v>
       </c>
-      <c r="M21" s="6"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
     </row>
     <row r="22" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E22" s="10"/>
-      <c r="F22" s="5">
-        <v>8</v>
-      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="9"/>
       <c r="G22" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>8</v>
@@ -946,51 +943,53 @@
         <v>2</v>
       </c>
       <c r="K22" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="L22" s="3">
         <v>0</v>
       </c>
-      <c r="M22" s="5"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
     </row>
     <row r="23" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E23" s="10"/>
-      <c r="F23" s="8"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="8">
+        <v>9</v>
+      </c>
       <c r="G23" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I23" s="3">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="J23" s="3">
         <v>2</v>
       </c>
       <c r="K23" s="3">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="L23" s="3">
         <v>0</v>
       </c>
       <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
     </row>
     <row r="24" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E24" s="10"/>
-      <c r="F24" s="6"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="10"/>
       <c r="G24" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I24" s="3">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="J24" s="3">
         <v>2</v>
@@ -999,16 +998,16 @@
         <v>0.5</v>
       </c>
       <c r="L24" s="3">
-        <v>0</v>
-      </c>
-      <c r="M24" s="6"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="M24" s="10"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
     </row>
     <row r="25" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E25" s="10"/>
-      <c r="F25" s="5">
-        <v>9</v>
+      <c r="E25" s="7"/>
+      <c r="F25" s="8">
+        <v>10</v>
       </c>
       <c r="G25" s="3">
         <v>1</v>
@@ -1017,24 +1016,26 @@
         <v>8</v>
       </c>
       <c r="I25" s="3">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J25" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K25" s="3">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="L25" s="3">
         <v>0</v>
       </c>
-      <c r="M25" s="5"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
+      <c r="M25" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
     </row>
     <row r="26" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E26" s="10"/>
-      <c r="F26" s="8"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="9"/>
       <c r="G26" s="3">
         <v>2</v>
       </c>
@@ -1042,24 +1043,24 @@
         <v>8</v>
       </c>
       <c r="I26" s="3">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="J26" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K26" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L26" s="3">
         <v>0</v>
       </c>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
     </row>
     <row r="27" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E27" s="10"/>
-      <c r="F27" s="6"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="9"/>
       <c r="G27" s="3">
         <v>3</v>
       </c>
@@ -1067,236 +1068,107 @@
         <v>8</v>
       </c>
       <c r="I27" s="3">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J27" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K27" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="L27" s="3">
-        <v>2</v>
-      </c>
-      <c r="M27" s="6"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
     </row>
     <row r="28" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E28" s="10"/>
-      <c r="F28" s="5">
-        <v>10</v>
-      </c>
-      <c r="G28" s="3">
-        <v>1</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I28" s="3">
-        <v>20</v>
-      </c>
-      <c r="J28" s="3">
-        <v>3</v>
-      </c>
-      <c r="K28" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L28" s="3">
-        <v>0</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
     </row>
     <row r="29" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E29" s="10"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="3">
-        <v>2</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I29" s="3">
-        <v>25</v>
-      </c>
-      <c r="J29" s="3">
-        <v>0</v>
-      </c>
-      <c r="K29" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L29" s="3">
-        <v>0</v>
-      </c>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
     </row>
     <row r="30" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E30" s="10"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="3">
-        <v>3</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I30" s="3">
-        <v>25</v>
-      </c>
-      <c r="J30" s="3">
-        <v>0</v>
-      </c>
-      <c r="K30" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="L30" s="3">
-        <v>0</v>
-      </c>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
     </row>
     <row r="31" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E31" s="10"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="3">
-        <v>4</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I31" s="3">
-        <v>15</v>
-      </c>
-      <c r="J31" s="3">
-        <v>0</v>
-      </c>
-      <c r="K31" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L31" s="3">
-        <v>0</v>
-      </c>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
     </row>
     <row r="32" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E32" s="11"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="3">
-        <v>5</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I32" s="3">
-        <v>30</v>
-      </c>
-      <c r="J32" s="3">
-        <v>0</v>
-      </c>
-      <c r="K32" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="L32" s="3">
-        <v>0</v>
-      </c>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-    </row>
-    <row r="33" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E33" s="3"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-    </row>
-    <row r="34" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E34" s="3"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
-    </row>
-    <row r="35" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E35" s="3"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="7"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
-    </row>
-    <row r="36" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E36" s="3"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="7"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
-    </row>
-    <row r="37" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E37" s="3"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="7"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="E8:E32"/>
-    <mergeCell ref="N8:N32"/>
-    <mergeCell ref="O8:O32"/>
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="M22:M24"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="E8:E27"/>
+    <mergeCell ref="N8:N27"/>
+    <mergeCell ref="O8:O27"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="M23:M24"/>
     <mergeCell ref="F25:F27"/>
     <mergeCell ref="M25:M27"/>
-    <mergeCell ref="F28:F32"/>
-    <mergeCell ref="M28:M32"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="F19:F20"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="M14:M17"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="F14:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>